<commit_message>
Add CSV input handling and refactor Excel processing script
</commit_message>
<xml_diff>
--- a/data_transformation/excel_files/before_sorting.xlsx
+++ b/data_transformation/excel_files/before_sorting.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\PN1PEPF00007E8A\EXCELCNV\8ccde3d8-abae-4e6d-ba2e-2826b9ad8c34\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lelin\Documents\GitHub\py_learn\data_transformation\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2643B5DD-15E1-437F-BE2C-BA7E0FE7CB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4008B0-4562-4D7A-A64F-AE301CC4CFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{7E210BE8-902B-4727-963C-DDE58C4F536F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7E210BE8-902B-4727-963C-DDE58C4F536F}"/>
   </bookViews>
   <sheets>
-    <sheet name="in" sheetId="1" r:id="rId1"/>
+    <sheet name="alamin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -249,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1087,9 +1087,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:64">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:64">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:64">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>

</xml_diff>